<commit_message>
Code cleaning and ipynb file
</commit_message>
<xml_diff>
--- a/Claims.xlsx
+++ b/Claims.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9677fb49b71d73c6/Documents/Engineering/2023/Project industry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breco\Documents\Code\Fact_verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2778" documentId="8_{CB2EEEEB-E697-439A-8CCD-C5A528D829D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C3CE3EE-EE03-4789-B30B-F6392544739D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD2651E-96D3-4506-9854-F0CF607CB8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3A788BA1-49EB-4D1A-9559-7E63FFFB85CE}"/>
   </bookViews>
@@ -4231,7 +4231,7 @@
   <dimension ref="A1:I914"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="F909" sqref="F909"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>